<commit_message>
Added JSON and removed duplicate damage
</commit_message>
<xml_diff>
--- a/scrapper/framedata.xlsx
+++ b/scrapper/framedata.xlsx
@@ -597,12 +597,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>40,40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -693,12 +693,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -889,12 +889,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>40,40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -985,12 +985,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1185,12 +1185,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>40,40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1285,12 +1285,12 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1381,12 +1381,12 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1481,12 +1481,12 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>30,30</t>
+          <t>30</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1581,12 +1581,12 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1677,12 +1677,12 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1753,12 +1753,12 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>50,50</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1825,12 +1825,12 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1897,12 +1897,12 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1969,12 +1969,12 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -2045,12 +2045,12 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>50,50</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2117,12 +2117,12 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2189,12 +2189,12 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2231,7 +2231,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2285,12 +2285,12 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>80,80</t>
+          <t>80</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2331,7 +2331,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2385,12 +2385,12 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2431,7 +2431,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2461,12 +2461,12 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2503,7 +2503,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2557,12 +2557,12 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2603,7 +2603,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2657,12 +2657,12 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>50,50</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2703,7 +2703,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2749,12 +2749,12 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2791,7 +2791,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2825,12 +2825,12 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>130,130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>170,170</t>
+          <t>170</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2867,7 +2867,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2901,12 +2901,12 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>140,140</t>
+          <t>140</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>170,170</t>
+          <t>170</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2943,7 +2943,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2997,12 +2997,12 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -3039,7 +3039,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -3201,12 +3201,12 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3247,7 +3247,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3827,7 +3827,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -4027,7 +4027,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -4427,7 +4427,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -4729,12 +4729,12 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>80,80</t>
+          <t>80</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -4775,7 +4775,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -4867,7 +4867,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -4893,12 +4893,12 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -4935,7 +4935,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -4973,12 +4973,12 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>140,140</t>
+          <t>140</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -5015,7 +5015,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -5053,12 +5053,12 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>160,160</t>
+          <t>160</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -5095,7 +5095,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -5133,12 +5133,12 @@
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -5175,7 +5175,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -5213,12 +5213,12 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -5255,7 +5255,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -5306,7 +5306,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -5351,7 +5351,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -5402,7 +5402,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -5447,7 +5447,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -5539,7 +5539,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -5581,12 +5581,12 @@
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>340,340</t>
+          <t>340</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
@@ -5627,7 +5627,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -5681,12 +5681,12 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>40,40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N59" t="inlineStr">
@@ -5723,7 +5723,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -5777,12 +5777,12 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N60" t="inlineStr">
@@ -5819,7 +5819,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -5919,7 +5919,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -5973,12 +5973,12 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>40,40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
@@ -6015,7 +6015,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -6069,12 +6069,12 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
@@ -6115,7 +6115,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -6215,7 +6215,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -6269,12 +6269,12 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>40,40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -6315,7 +6315,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -6369,12 +6369,12 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
@@ -6411,7 +6411,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -6465,12 +6465,12 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -6511,7 +6511,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -6565,12 +6565,12 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>30,30</t>
+          <t>30</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N68" t="inlineStr">
@@ -6611,7 +6611,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -6665,12 +6665,12 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
@@ -6707,7 +6707,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -6761,12 +6761,12 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
@@ -6807,7 +6807,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -6837,12 +6837,12 @@
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr">
         <is>
-          <t>50,50</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
@@ -6879,7 +6879,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -6909,12 +6909,12 @@
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
@@ -6951,7 +6951,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -6981,12 +6981,12 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N73" t="inlineStr">
@@ -7023,7 +7023,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -7053,12 +7053,12 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N74" t="inlineStr">
@@ -7099,7 +7099,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -7129,12 +7129,12 @@
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr">
         <is>
-          <t>50,50</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
@@ -7171,7 +7171,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -7201,12 +7201,12 @@
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -7243,7 +7243,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -7273,12 +7273,12 @@
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
@@ -7315,7 +7315,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -7369,12 +7369,12 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>80,80</t>
+          <t>80</t>
         </is>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
@@ -7415,7 +7415,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -7469,12 +7469,12 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>90,90</t>
+          <t>90</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
@@ -7515,7 +7515,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -7545,12 +7545,12 @@
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
@@ -7587,7 +7587,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -7641,12 +7641,12 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -7687,7 +7687,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -7741,12 +7741,12 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>50,50</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="N82" t="inlineStr">
@@ -7787,7 +7787,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -7833,12 +7833,12 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>70,70</t>
+          <t>70</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N83" t="inlineStr">
@@ -7875,7 +7875,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -7909,12 +7909,12 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>130,130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>170,170</t>
+          <t>170</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
@@ -7951,7 +7951,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -7985,12 +7985,12 @@
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr">
         <is>
-          <t>140,140</t>
+          <t>140</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>170,170</t>
+          <t>170</t>
         </is>
       </c>
       <c r="N85" t="inlineStr">
@@ -8027,7 +8027,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -8081,12 +8081,12 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -8123,7 +8123,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -8179,7 +8179,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -8243,7 +8243,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -8285,12 +8285,12 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr">
         <is>
-          <t>60,60</t>
+          <t>60</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
@@ -8331,7 +8331,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -8427,7 +8427,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -8523,7 +8523,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -8619,7 +8619,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -8711,7 +8711,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -8911,7 +8911,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -9011,7 +9011,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -9111,7 +9111,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -9211,7 +9211,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -9311,7 +9311,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -9411,7 +9411,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -9511,7 +9511,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -9603,7 +9603,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -9695,7 +9695,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -9787,7 +9787,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -9813,12 +9813,12 @@
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr">
         <is>
-          <t>80,80</t>
+          <t>80</t>
         </is>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>120,120</t>
+          <t>120</t>
         </is>
       </c>
       <c r="N105" t="inlineStr">
@@ -9859,7 +9859,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -9951,7 +9951,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -9977,12 +9977,12 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr">
         <is>
-          <t>100,100</t>
+          <t>100</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>150,150</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N107" t="inlineStr">
@@ -10019,7 +10019,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -10057,12 +10057,12 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr">
         <is>
-          <t>140,140</t>
+          <t>140</t>
         </is>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -10099,7 +10099,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -10137,12 +10137,12 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr">
         <is>
-          <t>160,160</t>
+          <t>160</t>
         </is>
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="N109" t="inlineStr">
@@ -10179,7 +10179,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -10217,12 +10217,12 @@
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>180,180</t>
+          <t>180</t>
         </is>
       </c>
       <c r="N110" t="inlineStr">
@@ -10259,7 +10259,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -10297,12 +10297,12 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
@@ -10339,7 +10339,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -10390,7 +10390,7 @@
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="N112" t="inlineStr">
@@ -10435,7 +10435,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -10486,7 +10486,7 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>200,200</t>
+          <t>200</t>
         </is>
       </c>
       <c r="N113" t="inlineStr">
@@ -10531,7 +10531,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -10623,7 +10623,7 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -10665,12 +10665,12 @@
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr">
         <is>
-          <t>340,340</t>
+          <t>340</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">

</xml_diff>